<commit_message>
Add inversion speed R file and updated spinning spreadsheet from cdhig
</commit_message>
<xml_diff>
--- a/Data-analysis/Spinning.xlsx
+++ b/Data-analysis/Spinning.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D8441C-74FE-46FC-96FF-A3F989A3C9E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09AF328-F27E-4B6F-996E-8324D07B9E9C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22272" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="75">
   <si>
     <t>Disk</t>
   </si>
@@ -359,9 +359,6 @@
     <t>20.05_8x3long_glossy_4mL</t>
   </si>
   <si>
-    <t>Moat</t>
-  </si>
-  <si>
     <t>Donor</t>
   </si>
   <si>
@@ -372,6 +369,27 @@
   </si>
   <si>
     <t>20.05_8x3long_0.75x9mm_glossy</t>
+  </si>
+  <si>
+    <t>Moat_glossy</t>
+  </si>
+  <si>
+    <t>control-5</t>
+  </si>
+  <si>
+    <t>control-4</t>
+  </si>
+  <si>
+    <t>control-3</t>
+  </si>
+  <si>
+    <t>spin-3</t>
+  </si>
+  <si>
+    <t>spin-4</t>
+  </si>
+  <si>
+    <t>spin-5</t>
   </si>
 </sst>
 </file>
@@ -439,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -454,6 +472,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3180,11 +3204,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:S137"/>
+  <dimension ref="A1:AD137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K137" sqref="K137"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA129" sqref="AA129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3200,10 +3224,10 @@
     <col min="12" max="12" width="8.88671875" style="9"/>
     <col min="13" max="14" width="9.109375" style="9"/>
     <col min="15" max="16" width="8.88671875" style="10"/>
-    <col min="18" max="18" width="17.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5546875" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -3211,7 +3235,7 @@
         <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3255,8 +3279,26 @@
       <c r="Q1" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43242</v>
       </c>
@@ -3307,7 +3349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43242</v>
       </c>
@@ -3333,7 +3375,7 @@
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43242</v>
       </c>
@@ -3359,7 +3401,7 @@
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>43242</v>
       </c>
@@ -3385,7 +3427,7 @@
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43242</v>
       </c>
@@ -3411,7 +3453,7 @@
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43242</v>
       </c>
@@ -3437,7 +3479,7 @@
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>43258</v>
       </c>
@@ -3477,7 +3519,7 @@
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>43258</v>
       </c>
@@ -3516,7 +3558,7 @@
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>43258</v>
       </c>
@@ -3555,7 +3597,7 @@
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>43258</v>
       </c>
@@ -3594,7 +3636,7 @@
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>43258</v>
       </c>
@@ -3633,7 +3675,7 @@
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>43258</v>
       </c>
@@ -3672,7 +3714,7 @@
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>43258</v>
       </c>
@@ -3711,7 +3753,7 @@
       <c r="O14" s="9"/>
       <c r="P14" s="9"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>43258</v>
       </c>
@@ -3750,7 +3792,7 @@
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>43264</v>
       </c>
@@ -6968,7 +7010,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>43349</v>
       </c>
@@ -7004,7 +7046,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>43349</v>
       </c>
@@ -7040,7 +7082,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>43564</v>
       </c>
@@ -7048,7 +7090,7 @@
         <v>1</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D115" t="s">
         <v>62</v>
@@ -7069,7 +7111,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>43564</v>
       </c>
@@ -7077,7 +7119,7 @@
         <v>2</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D116" t="s">
         <v>63</v>
@@ -7098,7 +7140,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>43564</v>
       </c>
@@ -7106,7 +7148,7 @@
         <v>3</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D117" t="s">
         <v>62</v>
@@ -7127,7 +7169,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>43564</v>
       </c>
@@ -7135,7 +7177,7 @@
         <v>4</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D118" t="s">
         <v>63</v>
@@ -7156,7 +7198,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>43564</v>
       </c>
@@ -7164,7 +7206,7 @@
         <v>5</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D119" t="s">
         <v>62</v>
@@ -7185,7 +7227,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>43564</v>
       </c>
@@ -7193,7 +7235,7 @@
         <v>6</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D120" t="s">
         <v>63</v>
@@ -7214,7 +7256,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>43564</v>
       </c>
@@ -7222,7 +7264,7 @@
         <v>2</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D121" t="s">
         <v>62</v>
@@ -7243,7 +7285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>43564</v>
       </c>
@@ -7251,7 +7293,7 @@
         <v>3</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D122" t="s">
         <v>63</v>
@@ -7272,7 +7314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>43564</v>
       </c>
@@ -7280,7 +7322,7 @@
         <v>4</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D123" t="s">
         <v>62</v>
@@ -7301,7 +7343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>43564</v>
       </c>
@@ -7309,7 +7351,7 @@
         <v>5</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D124" t="s">
         <v>63</v>
@@ -7330,36 +7372,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A125" s="1">
+    <row r="125" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="14">
         <v>43564</v>
       </c>
-      <c r="B125" s="2">
+      <c r="B125" s="15">
         <v>6</v>
       </c>
-      <c r="C125" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D125" t="s">
+      <c r="C125" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D125" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E125">
-        <v>4</v>
-      </c>
-      <c r="F125" t="s">
+      <c r="E125" s="16">
+        <v>4</v>
+      </c>
+      <c r="F125" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G125" s="6">
+      <c r="G125" s="17">
         <v>0.4</v>
       </c>
-      <c r="K125" s="10">
+      <c r="H125" s="17"/>
+      <c r="I125" s="17"/>
+      <c r="J125" s="17"/>
+      <c r="K125" s="18">
         <v>4.0335000000000001</v>
       </c>
-      <c r="L125" s="9">
+      <c r="L125" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M125" s="13"/>
+      <c r="N125" s="13"/>
+      <c r="O125" s="18"/>
+      <c r="P125" s="18"/>
+      <c r="R125" s="18"/>
+    </row>
+    <row r="126" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>43571</v>
       </c>
@@ -7367,10 +7417,10 @@
         <v>1</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D126" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E126">
         <v>4</v>
@@ -7381,6 +7431,7 @@
       <c r="G126" s="6">
         <v>0.4</v>
       </c>
+      <c r="H126" s="10"/>
       <c r="K126" s="10">
         <f>10.2453-6.0653</f>
         <v>4.1800000000000006</v>
@@ -7388,8 +7439,51 @@
       <c r="L126" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S126">
+        <v>239</v>
+      </c>
+      <c r="T126">
+        <v>25</v>
+      </c>
+      <c r="U126">
+        <v>411</v>
+      </c>
+      <c r="V126">
+        <v>48</v>
+      </c>
+      <c r="W126">
+        <v>7</v>
+      </c>
+      <c r="X126" s="19">
+        <f>R126/50*1000*10^3</f>
+        <v>0</v>
+      </c>
+      <c r="Y126" s="19">
+        <f>S126/50*1000*10^4</f>
+        <v>47800000</v>
+      </c>
+      <c r="Z126" s="19">
+        <f>T126/50*1000*10^5</f>
+        <v>50000000</v>
+      </c>
+      <c r="AA126" s="19">
+        <f>U126/50*1000*10^3</f>
+        <v>8220000</v>
+      </c>
+      <c r="AB126" s="19">
+        <f>V126/50*1000*10^4</f>
+        <v>9600000</v>
+      </c>
+      <c r="AC126" s="19">
+        <f>W126/50*1000*10^5</f>
+        <v>14000000</v>
+      </c>
+      <c r="AD126" s="19">
+        <f>AA126*K126/(Y126*7)</f>
+        <v>0.10268858338314407</v>
+      </c>
+    </row>
+    <row r="127" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>43571</v>
       </c>
@@ -7397,10 +7491,10 @@
         <v>2</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D127" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E127">
         <v>4</v>
@@ -7411,6 +7505,7 @@
       <c r="G127" s="6">
         <v>0.4</v>
       </c>
+      <c r="H127" s="10"/>
       <c r="K127" s="10">
         <f>10.2162-6.1252</f>
         <v>4.0910000000000002</v>
@@ -7418,8 +7513,51 @@
       <c r="L127" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S127">
+        <v>206</v>
+      </c>
+      <c r="T127">
+        <v>33</v>
+      </c>
+      <c r="U127">
+        <v>490</v>
+      </c>
+      <c r="V127">
+        <v>74</v>
+      </c>
+      <c r="W127">
+        <v>4</v>
+      </c>
+      <c r="X127" s="19">
+        <f>R127/50*1000*10^3</f>
+        <v>0</v>
+      </c>
+      <c r="Y127" s="19">
+        <f t="shared" ref="Y126:Y128" si="3">S127/50*1000*10^4</f>
+        <v>41200000</v>
+      </c>
+      <c r="Z127" s="19">
+        <f>T127/50*1000*10^5</f>
+        <v>66000000</v>
+      </c>
+      <c r="AA127" s="19">
+        <f>U127/50*1000*10^3</f>
+        <v>9800000</v>
+      </c>
+      <c r="AB127" s="19">
+        <f>V127/50*1000*10^4</f>
+        <v>14800000</v>
+      </c>
+      <c r="AC127" s="19">
+        <f>W127/50*1000*10^5</f>
+        <v>8000000</v>
+      </c>
+      <c r="AD127" s="19">
+        <f t="shared" ref="AD127:AD137" si="4">AA127*K127/(Y127*7)</f>
+        <v>0.13901456310679611</v>
+      </c>
+    </row>
+    <row r="128" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>43571</v>
       </c>
@@ -7427,7 +7565,7 @@
         <v>3</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D128" t="s">
         <v>58</v>
@@ -7441,6 +7579,7 @@
       <c r="G128" s="6">
         <v>0.4</v>
       </c>
+      <c r="H128" s="10"/>
       <c r="K128" s="10">
         <f>10.2255-6.08</f>
         <v>4.1455000000000002</v>
@@ -7448,8 +7587,51 @@
       <c r="L128" s="9">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S128">
+        <v>276</v>
+      </c>
+      <c r="T128">
+        <v>29</v>
+      </c>
+      <c r="U128">
+        <v>486</v>
+      </c>
+      <c r="V128">
+        <v>87</v>
+      </c>
+      <c r="W128">
+        <v>6</v>
+      </c>
+      <c r="X128" s="19">
+        <f>R128/50*1000*10^3</f>
+        <v>0</v>
+      </c>
+      <c r="Y128" s="19">
+        <f t="shared" si="3"/>
+        <v>55200000</v>
+      </c>
+      <c r="Z128" s="19">
+        <f>T128/50*1000*10^5</f>
+        <v>58000000</v>
+      </c>
+      <c r="AA128" s="19">
+        <f>U128/50*1000*10^3</f>
+        <v>9720000</v>
+      </c>
+      <c r="AB128" s="19">
+        <f>V128/50*1000*10^4</f>
+        <v>17400000</v>
+      </c>
+      <c r="AC128" s="19">
+        <f>W128/50*1000*10^5</f>
+        <v>12000000</v>
+      </c>
+      <c r="AD128" s="19">
+        <f t="shared" si="4"/>
+        <v>0.10428121118012422</v>
+      </c>
+    </row>
+    <row r="129" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>43571</v>
       </c>
@@ -7457,10 +7639,10 @@
         <v>4</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D129" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E129">
         <v>4</v>
@@ -7471,6 +7653,7 @@
       <c r="G129" s="6">
         <v>0.4</v>
       </c>
+      <c r="H129" s="10"/>
       <c r="K129" s="10">
         <f>9.8478-6.0909</f>
         <v>3.756899999999999</v>
@@ -7478,8 +7661,51 @@
       <c r="L129" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="S129">
+        <v>229</v>
+      </c>
+      <c r="T129">
+        <v>26</v>
+      </c>
+      <c r="U129">
+        <v>496</v>
+      </c>
+      <c r="V129">
+        <v>67</v>
+      </c>
+      <c r="W129">
+        <v>6</v>
+      </c>
+      <c r="X129" s="19">
+        <f>R129/50*1000*10^3</f>
+        <v>0</v>
+      </c>
+      <c r="Y129" s="19">
+        <f>S129/50*1000*10^4</f>
+        <v>45800000</v>
+      </c>
+      <c r="Z129" s="19">
+        <f>T129/50*1000*10^5</f>
+        <v>52000000</v>
+      </c>
+      <c r="AA129" s="19">
+        <f>U129/50*1000*10^3</f>
+        <v>9920000</v>
+      </c>
+      <c r="AB129" s="19">
+        <f>V129/50*1000*10^4</f>
+        <v>13400000</v>
+      </c>
+      <c r="AC129" s="19">
+        <f>W129/50*1000*10^5</f>
+        <v>12000000</v>
+      </c>
+      <c r="AD129" s="19">
+        <f t="shared" si="4"/>
+        <v>0.11624593886462879</v>
+      </c>
+    </row>
+    <row r="130" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>43571</v>
       </c>
@@ -7487,10 +7713,10 @@
         <v>5</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D130" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E130">
         <v>4</v>
@@ -7501,6 +7727,7 @@
       <c r="G130" s="6">
         <v>0.4</v>
       </c>
+      <c r="H130" s="10"/>
       <c r="K130" s="10">
         <f>10.0103-5.9315</f>
         <v>4.0788000000000011</v>
@@ -7508,8 +7735,54 @@
       <c r="L130" s="9">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="R130" s="10">
+        <v>774</v>
+      </c>
+      <c r="S130">
+        <v>222</v>
+      </c>
+      <c r="T130">
+        <v>31</v>
+      </c>
+      <c r="U130">
+        <v>489</v>
+      </c>
+      <c r="V130">
+        <v>66</v>
+      </c>
+      <c r="W130">
+        <v>9</v>
+      </c>
+      <c r="X130" s="19">
+        <f>R130/50*1000*10^3</f>
+        <v>15480000</v>
+      </c>
+      <c r="Y130" s="19">
+        <f>S130/50*1000*10^4</f>
+        <v>44400000</v>
+      </c>
+      <c r="Z130" s="19">
+        <f>T130/50*1000*10^5</f>
+        <v>62000000</v>
+      </c>
+      <c r="AA130" s="19">
+        <f>U130/50*1000*10^3</f>
+        <v>9780000</v>
+      </c>
+      <c r="AB130" s="19">
+        <f>V130/50*1000*10^4</f>
+        <v>13200000</v>
+      </c>
+      <c r="AC130" s="19">
+        <f>W130/50*1000*10^5</f>
+        <v>18000000</v>
+      </c>
+      <c r="AD130" s="19">
+        <f t="shared" si="4"/>
+        <v>0.12834833976833979</v>
+      </c>
+    </row>
+    <row r="131" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>43571</v>
       </c>
@@ -7517,7 +7790,7 @@
         <v>6</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D131" t="s">
         <v>58</v>
@@ -7531,6 +7804,7 @@
       <c r="G131" s="6">
         <v>0.4</v>
       </c>
+      <c r="H131" s="10"/>
       <c r="K131" s="10">
         <f>10.37-6.0706</f>
         <v>4.2993999999999994</v>
@@ -7538,8 +7812,54 @@
       <c r="L131" s="9">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="R131" s="10">
+        <v>750</v>
+      </c>
+      <c r="S131">
+        <v>198</v>
+      </c>
+      <c r="T131">
+        <v>18</v>
+      </c>
+      <c r="U131">
+        <v>429</v>
+      </c>
+      <c r="V131">
+        <v>72</v>
+      </c>
+      <c r="W131">
+        <v>5</v>
+      </c>
+      <c r="X131" s="19">
+        <f>R131/50*1000*10^3</f>
+        <v>15000000</v>
+      </c>
+      <c r="Y131" s="19">
+        <f>S131/50*1000*10^4</f>
+        <v>39600000</v>
+      </c>
+      <c r="Z131" s="19">
+        <f>T131/50*1000*10^5</f>
+        <v>36000000</v>
+      </c>
+      <c r="AA131" s="19">
+        <f>U131/50*1000*10^3</f>
+        <v>8580000</v>
+      </c>
+      <c r="AB131" s="19">
+        <f>V131/50*1000*10^4</f>
+        <v>14400000</v>
+      </c>
+      <c r="AC131" s="19">
+        <f>W131/50*1000*10^5</f>
+        <v>10000000</v>
+      </c>
+      <c r="AD131" s="19">
+        <f t="shared" si="4"/>
+        <v>0.13307666666666665</v>
+      </c>
+    </row>
+    <row r="132" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>43571</v>
       </c>
@@ -7547,7 +7867,7 @@
         <v>1</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D132" t="s">
         <v>58</v>
@@ -7561,6 +7881,7 @@
       <c r="G132" s="6">
         <v>0.45</v>
       </c>
+      <c r="H132" s="10"/>
       <c r="K132" s="10">
         <f>10.042-6.0564</f>
         <v>3.9855999999999998</v>
@@ -7568,8 +7889,45 @@
       <c r="L132" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U132">
+        <v>392</v>
+      </c>
+      <c r="V132">
+        <v>42</v>
+      </c>
+      <c r="W132">
+        <v>4</v>
+      </c>
+      <c r="X132" s="19">
+        <f>R132/50*1000*10^3</f>
+        <v>0</v>
+      </c>
+      <c r="Y132" s="19">
+        <f>S132/50*1000*10^4</f>
+        <v>0</v>
+      </c>
+      <c r="Z132" s="19">
+        <f>T132/50*1000*10^5</f>
+        <v>0</v>
+      </c>
+      <c r="AA132" s="19">
+        <f>U132/50*1000*10^3</f>
+        <v>7840000</v>
+      </c>
+      <c r="AB132" s="19">
+        <f>V132/50*1000*10^4</f>
+        <v>8400000</v>
+      </c>
+      <c r="AC132" s="19">
+        <f>W132/50*1000*10^5</f>
+        <v>8000000</v>
+      </c>
+      <c r="AD132" s="19" t="e">
+        <f>AA132*K132/(Y132*7)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="133" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>43571</v>
       </c>
@@ -7577,10 +7935,10 @@
         <v>2</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D133" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E133">
         <v>4</v>
@@ -7591,6 +7949,7 @@
       <c r="G133" s="6">
         <v>0.45</v>
       </c>
+      <c r="H133" s="10"/>
       <c r="K133" s="10">
         <f>9.8601-6.0358</f>
         <v>3.8242999999999991</v>
@@ -7598,8 +7957,45 @@
       <c r="L133" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U133">
+        <v>421</v>
+      </c>
+      <c r="V133">
+        <v>56</v>
+      </c>
+      <c r="W133">
+        <v>3</v>
+      </c>
+      <c r="X133" s="19">
+        <f>R133/50*1000*10^3</f>
+        <v>0</v>
+      </c>
+      <c r="Y133" s="19">
+        <f>S133/50*1000*10^4</f>
+        <v>0</v>
+      </c>
+      <c r="Z133" s="19">
+        <f>T133/50*1000*10^5</f>
+        <v>0</v>
+      </c>
+      <c r="AA133" s="19">
+        <f>U133/50*1000*10^3</f>
+        <v>8420000</v>
+      </c>
+      <c r="AB133" s="19">
+        <f>V133/50*1000*10^4</f>
+        <v>11200000</v>
+      </c>
+      <c r="AC133" s="19">
+        <f>W133/50*1000*10^5</f>
+        <v>6000000</v>
+      </c>
+      <c r="AD133" s="19" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="134" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>43571</v>
       </c>
@@ -7607,10 +8003,10 @@
         <v>3</v>
       </c>
       <c r="C134" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D134" t="s">
         <v>67</v>
-      </c>
-      <c r="D134" t="s">
-        <v>68</v>
       </c>
       <c r="E134">
         <v>4</v>
@@ -7621,6 +8017,7 @@
       <c r="G134" s="6">
         <v>0.45</v>
       </c>
+      <c r="H134" s="10"/>
       <c r="K134" s="10">
         <f>10.3403-6.0875</f>
         <v>4.2527999999999988</v>
@@ -7628,8 +8025,45 @@
       <c r="L134" s="9">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U134">
+        <v>466</v>
+      </c>
+      <c r="V134">
+        <v>77</v>
+      </c>
+      <c r="W134">
+        <v>7</v>
+      </c>
+      <c r="X134" s="19">
+        <f>R134/50*1000*10^3</f>
+        <v>0</v>
+      </c>
+      <c r="Y134" s="19">
+        <f>S134/50*1000*10^4</f>
+        <v>0</v>
+      </c>
+      <c r="Z134" s="19">
+        <f>T134/50*1000*10^5</f>
+        <v>0</v>
+      </c>
+      <c r="AA134" s="19">
+        <f>U134/50*1000*10^3</f>
+        <v>9320000</v>
+      </c>
+      <c r="AB134" s="19">
+        <f>V134/50*1000*10^4</f>
+        <v>15400000</v>
+      </c>
+      <c r="AC134" s="19">
+        <f>W134/50*1000*10^5</f>
+        <v>14000000</v>
+      </c>
+      <c r="AD134" s="19" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="135" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>43571</v>
       </c>
@@ -7637,7 +8071,7 @@
         <v>4</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D135" t="s">
         <v>58</v>
@@ -7651,6 +8085,7 @@
       <c r="G135" s="6">
         <v>0.45</v>
       </c>
+      <c r="H135" s="10"/>
       <c r="K135" s="10">
         <f>9.87-6.0185</f>
         <v>3.8514999999999988</v>
@@ -7658,8 +8093,45 @@
       <c r="L135" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U135">
+        <v>417</v>
+      </c>
+      <c r="V135">
+        <v>76</v>
+      </c>
+      <c r="W135">
+        <v>7</v>
+      </c>
+      <c r="X135" s="19">
+        <f>R135/50*1000*10^3</f>
+        <v>0</v>
+      </c>
+      <c r="Y135" s="19">
+        <f>S135/50*1000*10^4</f>
+        <v>0</v>
+      </c>
+      <c r="Z135" s="19">
+        <f>T135/50*1000*10^5</f>
+        <v>0</v>
+      </c>
+      <c r="AA135" s="19">
+        <f>U135/50*1000*10^3</f>
+        <v>8340000</v>
+      </c>
+      <c r="AB135" s="19">
+        <f>V135/50*1000*10^4</f>
+        <v>15200000</v>
+      </c>
+      <c r="AC135" s="19">
+        <f>W135/50*1000*10^5</f>
+        <v>14000000</v>
+      </c>
+      <c r="AD135" s="19" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="136" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>43571</v>
       </c>
@@ -7667,10 +8139,10 @@
         <v>5</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D136" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E136">
         <v>4</v>
@@ -7681,6 +8153,7 @@
       <c r="G136" s="6">
         <v>0.45</v>
       </c>
+      <c r="H136" s="10"/>
       <c r="K136" s="10">
         <f>9.7643-6.1272</f>
         <v>3.6371000000000002</v>
@@ -7688,8 +8161,45 @@
       <c r="L136" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U136">
+        <v>362</v>
+      </c>
+      <c r="V136">
+        <v>56</v>
+      </c>
+      <c r="W136">
+        <v>7</v>
+      </c>
+      <c r="X136" s="19">
+        <f>R136/50*1000*10^3</f>
+        <v>0</v>
+      </c>
+      <c r="Y136" s="19">
+        <f>S136/50*1000*10^4</f>
+        <v>0</v>
+      </c>
+      <c r="Z136" s="19">
+        <f>T136/50*1000*10^5</f>
+        <v>0</v>
+      </c>
+      <c r="AA136" s="19">
+        <f>U136/50*1000*10^3</f>
+        <v>7240000</v>
+      </c>
+      <c r="AB136" s="19">
+        <f>V136/50*1000*10^4</f>
+        <v>11200000</v>
+      </c>
+      <c r="AC136" s="19">
+        <f>W136/50*1000*10^5</f>
+        <v>14000000</v>
+      </c>
+      <c r="AD136" s="19" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="137" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>43571</v>
       </c>
@@ -7697,10 +8207,10 @@
         <v>6</v>
       </c>
       <c r="C137" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D137" t="s">
         <v>67</v>
-      </c>
-      <c r="D137" t="s">
-        <v>68</v>
       </c>
       <c r="E137">
         <v>4</v>
@@ -7711,12 +8221,50 @@
       <c r="G137" s="6">
         <v>0.45</v>
       </c>
+      <c r="H137" s="10"/>
       <c r="K137" s="10">
         <f>10.2479-6.1058</f>
         <v>4.1420999999999992</v>
       </c>
       <c r="L137" s="9">
         <v>1E-3</v>
+      </c>
+      <c r="U137">
+        <v>404</v>
+      </c>
+      <c r="V137">
+        <v>60</v>
+      </c>
+      <c r="W137">
+        <v>5</v>
+      </c>
+      <c r="X137" s="19">
+        <f>R137/50*1000*10^3</f>
+        <v>0</v>
+      </c>
+      <c r="Y137" s="19">
+        <f>S137/50*1000*10^4</f>
+        <v>0</v>
+      </c>
+      <c r="Z137" s="19">
+        <f>T137/50*1000*10^5</f>
+        <v>0</v>
+      </c>
+      <c r="AA137" s="19">
+        <f>U137/50*1000*10^3</f>
+        <v>8080000</v>
+      </c>
+      <c r="AB137" s="19">
+        <f>V137/50*1000*10^4</f>
+        <v>12000000</v>
+      </c>
+      <c r="AC137" s="19">
+        <f>W137/50*1000*10^5</f>
+        <v>10000000</v>
+      </c>
+      <c r="AD137" s="19" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculate dilution values, update spinning spreadsheet with second half of bacterial recoveries from moat, discard changes to velocity_functions
</commit_message>
<xml_diff>
--- a/Data-analysis/Spinning.xlsx
+++ b/Data-analysis/Spinning.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09AF328-F27E-4B6F-996E-8324D07B9E9C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D218B502-5D7D-49A9-A65F-E248D68764CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22272" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22272" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_page_wide" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="82">
   <si>
     <t>Disk</t>
   </si>
@@ -390,6 +390,27 @@
   </si>
   <si>
     <t>spin-5</t>
+  </si>
+  <si>
+    <t>bac_recovery</t>
+  </si>
+  <si>
+    <t>c_control-3</t>
+  </si>
+  <si>
+    <t>c_control-4</t>
+  </si>
+  <si>
+    <t>c_control-5</t>
+  </si>
+  <si>
+    <t>c_spin-3</t>
+  </si>
+  <si>
+    <t>c_spin-4</t>
+  </si>
+  <si>
+    <t>c_spin-5</t>
   </si>
 </sst>
 </file>
@@ -1687,15 +1708,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>398145</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>188595</xdr:rowOff>
+      <xdr:colOff>596265</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>120015</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>207945</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>66886</xdr:rowOff>
+      <xdr:colOff>406065</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>5926</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1724,8 +1745,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5274945" y="4189095"/>
-          <a:ext cx="3353100" cy="2545291"/>
+          <a:off x="6265545" y="3228975"/>
+          <a:ext cx="3467400" cy="2446231"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1736,16 +1757,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>543233</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>139373</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>541019</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>65123</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>137159</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>179423</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1774,8 +1795,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5420033" y="6753225"/>
-          <a:ext cx="3541086" cy="3027398"/>
+          <a:off x="6418253" y="5869305"/>
+          <a:ext cx="3655386" cy="2905478"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2147,7 +2168,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="I8" sqref="I8:I15"/>
     </sheetView>
   </sheetViews>
@@ -3206,9 +3227,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AD137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA129" sqref="AA129"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z131" sqref="Z131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3225,9 +3246,10 @@
     <col min="13" max="14" width="9.109375" style="9"/>
     <col min="15" max="16" width="8.88671875" style="10"/>
     <col min="18" max="18" width="8.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="29" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -3297,8 +3319,29 @@
       <c r="W1" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43242</v>
       </c>
@@ -3349,7 +3392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43242</v>
       </c>
@@ -3375,7 +3418,7 @@
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43242</v>
       </c>
@@ -3401,7 +3444,7 @@
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>43242</v>
       </c>
@@ -3427,7 +3470,7 @@
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43242</v>
       </c>
@@ -3453,7 +3496,7 @@
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43242</v>
       </c>
@@ -3479,7 +3522,7 @@
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>43258</v>
       </c>
@@ -3519,7 +3562,7 @@
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>43258</v>
       </c>
@@ -3558,7 +3601,7 @@
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>43258</v>
       </c>
@@ -3597,7 +3640,7 @@
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>43258</v>
       </c>
@@ -3636,7 +3679,7 @@
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>43258</v>
       </c>
@@ -3675,7 +3718,7 @@
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>43258</v>
       </c>
@@ -3714,7 +3757,7 @@
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>43258</v>
       </c>
@@ -3753,7 +3796,7 @@
       <c r="O14" s="9"/>
       <c r="P14" s="9"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>43258</v>
       </c>
@@ -3792,7 +3835,7 @@
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>43264</v>
       </c>
@@ -7463,22 +7506,22 @@
         <v>47800000</v>
       </c>
       <c r="Z126" s="19">
-        <f>T126/50*1000*10^5</f>
+        <f t="shared" ref="Z126:Z137" si="3">T126/50*1000*10^5</f>
         <v>50000000</v>
       </c>
       <c r="AA126" s="19">
-        <f>U126/50*1000*10^3</f>
+        <f t="shared" ref="AA126:AA137" si="4">U126/50*1000*10^3</f>
         <v>8220000</v>
       </c>
       <c r="AB126" s="19">
-        <f>V126/50*1000*10^4</f>
+        <f t="shared" ref="AB126:AB137" si="5">V126/50*1000*10^4</f>
         <v>9600000</v>
       </c>
       <c r="AC126" s="19">
-        <f>W126/50*1000*10^5</f>
+        <f t="shared" ref="AC126:AC137" si="6">W126/50*1000*10^5</f>
         <v>14000000</v>
       </c>
-      <c r="AD126" s="19">
+      <c r="AD126" s="6">
         <f>AA126*K126/(Y126*7)</f>
         <v>0.10268858338314407</v>
       </c>
@@ -7529,31 +7572,31 @@
         <v>4</v>
       </c>
       <c r="X127" s="19">
-        <f>R127/50*1000*10^3</f>
+        <f t="shared" ref="X126:X137" si="7">R127/50*1000*10^3</f>
         <v>0</v>
       </c>
       <c r="Y127" s="19">
-        <f t="shared" ref="Y126:Y128" si="3">S127/50*1000*10^4</f>
+        <f t="shared" ref="Y127:Y128" si="8">S127/50*1000*10^4</f>
         <v>41200000</v>
       </c>
       <c r="Z127" s="19">
-        <f>T127/50*1000*10^5</f>
+        <f t="shared" si="3"/>
         <v>66000000</v>
       </c>
       <c r="AA127" s="19">
-        <f>U127/50*1000*10^3</f>
+        <f t="shared" si="4"/>
         <v>9800000</v>
       </c>
       <c r="AB127" s="19">
-        <f>V127/50*1000*10^4</f>
+        <f t="shared" si="5"/>
         <v>14800000</v>
       </c>
       <c r="AC127" s="19">
-        <f>W127/50*1000*10^5</f>
+        <f t="shared" si="6"/>
         <v>8000000</v>
       </c>
-      <c r="AD127" s="19">
-        <f t="shared" ref="AD127:AD137" si="4">AA127*K127/(Y127*7)</f>
+      <c r="AD127" s="6">
+        <f t="shared" ref="AD127:AD137" si="9">AA127*K127/(Y127*7)</f>
         <v>0.13901456310679611</v>
       </c>
     </row>
@@ -7603,31 +7646,31 @@
         <v>6</v>
       </c>
       <c r="X128" s="19">
-        <f>R128/50*1000*10^3</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y128" s="19">
+        <f t="shared" si="8"/>
+        <v>55200000</v>
+      </c>
+      <c r="Z128" s="19">
         <f t="shared" si="3"/>
-        <v>55200000</v>
-      </c>
-      <c r="Z128" s="19">
-        <f>T128/50*1000*10^5</f>
         <v>58000000</v>
       </c>
       <c r="AA128" s="19">
-        <f>U128/50*1000*10^3</f>
+        <f t="shared" si="4"/>
         <v>9720000</v>
       </c>
       <c r="AB128" s="19">
-        <f>V128/50*1000*10^4</f>
+        <f t="shared" si="5"/>
         <v>17400000</v>
       </c>
       <c r="AC128" s="19">
-        <f>W128/50*1000*10^5</f>
+        <f t="shared" si="6"/>
         <v>12000000</v>
       </c>
-      <c r="AD128" s="19">
-        <f t="shared" si="4"/>
+      <c r="AD128" s="6">
+        <f t="shared" si="9"/>
         <v>0.10428121118012422</v>
       </c>
     </row>
@@ -7677,31 +7720,31 @@
         <v>6</v>
       </c>
       <c r="X129" s="19">
-        <f>R129/50*1000*10^3</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y129" s="19">
-        <f>S129/50*1000*10^4</f>
+        <f t="shared" ref="Y129:Y137" si="10">S129/50*1000*10^4</f>
         <v>45800000</v>
       </c>
       <c r="Z129" s="19">
-        <f>T129/50*1000*10^5</f>
+        <f t="shared" si="3"/>
         <v>52000000</v>
       </c>
       <c r="AA129" s="19">
-        <f>U129/50*1000*10^3</f>
+        <f t="shared" si="4"/>
         <v>9920000</v>
       </c>
       <c r="AB129" s="19">
-        <f>V129/50*1000*10^4</f>
+        <f t="shared" si="5"/>
         <v>13400000</v>
       </c>
       <c r="AC129" s="19">
-        <f>W129/50*1000*10^5</f>
+        <f t="shared" si="6"/>
         <v>12000000</v>
       </c>
-      <c r="AD129" s="19">
-        <f t="shared" si="4"/>
+      <c r="AD129" s="6">
+        <f t="shared" si="9"/>
         <v>0.11624593886462879</v>
       </c>
     </row>
@@ -7754,31 +7797,31 @@
         <v>9</v>
       </c>
       <c r="X130" s="19">
-        <f>R130/50*1000*10^3</f>
+        <f t="shared" si="7"/>
         <v>15480000</v>
       </c>
       <c r="Y130" s="19">
-        <f>S130/50*1000*10^4</f>
+        <f t="shared" si="10"/>
         <v>44400000</v>
       </c>
       <c r="Z130" s="19">
-        <f>T130/50*1000*10^5</f>
+        <f t="shared" si="3"/>
         <v>62000000</v>
       </c>
       <c r="AA130" s="19">
-        <f>U130/50*1000*10^3</f>
+        <f t="shared" si="4"/>
         <v>9780000</v>
       </c>
       <c r="AB130" s="19">
-        <f>V130/50*1000*10^4</f>
+        <f t="shared" si="5"/>
         <v>13200000</v>
       </c>
       <c r="AC130" s="19">
-        <f>W130/50*1000*10^5</f>
+        <f t="shared" si="6"/>
         <v>18000000</v>
       </c>
-      <c r="AD130" s="19">
-        <f t="shared" si="4"/>
+      <c r="AD130" s="6">
+        <f t="shared" si="9"/>
         <v>0.12834833976833979</v>
       </c>
     </row>
@@ -7831,31 +7874,31 @@
         <v>5</v>
       </c>
       <c r="X131" s="19">
-        <f>R131/50*1000*10^3</f>
+        <f t="shared" si="7"/>
         <v>15000000</v>
       </c>
       <c r="Y131" s="19">
-        <f>S131/50*1000*10^4</f>
+        <f t="shared" si="10"/>
         <v>39600000</v>
       </c>
       <c r="Z131" s="19">
-        <f>T131/50*1000*10^5</f>
+        <f t="shared" si="3"/>
         <v>36000000</v>
       </c>
       <c r="AA131" s="19">
-        <f>U131/50*1000*10^3</f>
+        <f t="shared" si="4"/>
         <v>8580000</v>
       </c>
       <c r="AB131" s="19">
-        <f>V131/50*1000*10^4</f>
+        <f t="shared" si="5"/>
         <v>14400000</v>
       </c>
       <c r="AC131" s="19">
-        <f>W131/50*1000*10^5</f>
+        <f t="shared" si="6"/>
         <v>10000000</v>
       </c>
-      <c r="AD131" s="19">
-        <f t="shared" si="4"/>
+      <c r="AD131" s="6">
+        <f t="shared" si="9"/>
         <v>0.13307666666666665</v>
       </c>
     </row>
@@ -7889,6 +7932,12 @@
       <c r="L132" s="9">
         <v>0</v>
       </c>
+      <c r="S132">
+        <v>123</v>
+      </c>
+      <c r="T132">
+        <v>14</v>
+      </c>
       <c r="U132">
         <v>392</v>
       </c>
@@ -7899,32 +7948,32 @@
         <v>4</v>
       </c>
       <c r="X132" s="19">
-        <f>R132/50*1000*10^3</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y132" s="19">
-        <f>S132/50*1000*10^4</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>24600000</v>
       </c>
       <c r="Z132" s="19">
-        <f>T132/50*1000*10^5</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>28000000</v>
       </c>
       <c r="AA132" s="19">
         <f>U132/50*1000*10^3</f>
         <v>7840000</v>
       </c>
       <c r="AB132" s="19">
-        <f>V132/50*1000*10^4</f>
+        <f t="shared" si="5"/>
         <v>8400000</v>
       </c>
       <c r="AC132" s="19">
-        <f>W132/50*1000*10^5</f>
+        <f t="shared" si="6"/>
         <v>8000000</v>
       </c>
-      <c r="AD132" s="19" t="e">
+      <c r="AD132" s="6">
         <f>AA132*K132/(Y132*7)</f>
-        <v>#DIV/0!</v>
+        <v>0.18145821138211382</v>
       </c>
     </row>
     <row r="133" spans="1:30" x14ac:dyDescent="0.3">
@@ -7957,6 +8006,12 @@
       <c r="L133" s="9">
         <v>0</v>
       </c>
+      <c r="S133">
+        <v>67</v>
+      </c>
+      <c r="T133">
+        <v>4</v>
+      </c>
       <c r="U133">
         <v>421</v>
       </c>
@@ -7967,32 +8022,32 @@
         <v>3</v>
       </c>
       <c r="X133" s="19">
-        <f>R133/50*1000*10^3</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y133" s="19">
-        <f>S133/50*1000*10^4</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>13400000</v>
       </c>
       <c r="Z133" s="19">
-        <f>T133/50*1000*10^5</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>8000000</v>
       </c>
       <c r="AA133" s="19">
-        <f>U133/50*1000*10^3</f>
+        <f t="shared" si="4"/>
         <v>8420000</v>
       </c>
       <c r="AB133" s="19">
-        <f>V133/50*1000*10^4</f>
+        <f t="shared" si="5"/>
         <v>11200000</v>
       </c>
       <c r="AC133" s="19">
-        <f>W133/50*1000*10^5</f>
+        <f t="shared" si="6"/>
         <v>6000000</v>
       </c>
-      <c r="AD133" s="19" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+      <c r="AD133" s="6">
+        <f>AA133*K133/(Y133*7)</f>
+        <v>0.34329004264392315</v>
       </c>
     </row>
     <row r="134" spans="1:30" x14ac:dyDescent="0.3">
@@ -8025,6 +8080,12 @@
       <c r="L134" s="9">
         <v>1E-3</v>
       </c>
+      <c r="S134">
+        <v>52</v>
+      </c>
+      <c r="T134">
+        <v>5</v>
+      </c>
       <c r="U134">
         <v>466</v>
       </c>
@@ -8035,32 +8096,32 @@
         <v>7</v>
       </c>
       <c r="X134" s="19">
-        <f>R134/50*1000*10^3</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y134" s="19">
-        <f>S134/50*1000*10^4</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>10400000</v>
       </c>
       <c r="Z134" s="19">
-        <f>T134/50*1000*10^5</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>10000000</v>
       </c>
       <c r="AA134" s="19">
-        <f>U134/50*1000*10^3</f>
+        <f t="shared" si="4"/>
         <v>9320000</v>
       </c>
       <c r="AB134" s="19">
-        <f>V134/50*1000*10^4</f>
+        <f t="shared" si="5"/>
         <v>15400000</v>
       </c>
       <c r="AC134" s="19">
-        <f>W134/50*1000*10^5</f>
+        <f t="shared" si="6"/>
         <v>14000000</v>
       </c>
-      <c r="AD134" s="19" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+      <c r="AD134" s="6">
+        <f>AA134*K134/(Y134*7)</f>
+        <v>0.54445186813186808</v>
       </c>
     </row>
     <row r="135" spans="1:30" x14ac:dyDescent="0.3">
@@ -8093,6 +8154,12 @@
       <c r="L135" s="9">
         <v>0</v>
       </c>
+      <c r="S135">
+        <v>75</v>
+      </c>
+      <c r="T135">
+        <v>33</v>
+      </c>
       <c r="U135">
         <v>417</v>
       </c>
@@ -8103,32 +8170,32 @@
         <v>7</v>
       </c>
       <c r="X135" s="19">
-        <f>R135/50*1000*10^3</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y135" s="19">
-        <f>S135/50*1000*10^4</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>15000000</v>
       </c>
       <c r="Z135" s="19">
-        <f>T135/50*1000*10^5</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>66000000</v>
       </c>
       <c r="AA135" s="19">
-        <f>U135/50*1000*10^3</f>
+        <f t="shared" si="4"/>
         <v>8340000</v>
       </c>
       <c r="AB135" s="19">
-        <f>V135/50*1000*10^4</f>
+        <f t="shared" si="5"/>
         <v>15200000</v>
       </c>
       <c r="AC135" s="19">
-        <f>W135/50*1000*10^5</f>
+        <f t="shared" si="6"/>
         <v>14000000</v>
       </c>
-      <c r="AD135" s="19" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+      <c r="AD135" s="6">
+        <f t="shared" si="9"/>
+        <v>0.30591914285714278</v>
       </c>
     </row>
     <row r="136" spans="1:30" x14ac:dyDescent="0.3">
@@ -8161,6 +8228,12 @@
       <c r="L136" s="9">
         <v>0</v>
       </c>
+      <c r="S136">
+        <v>98</v>
+      </c>
+      <c r="T136">
+        <v>5</v>
+      </c>
       <c r="U136">
         <v>362</v>
       </c>
@@ -8171,32 +8244,32 @@
         <v>7</v>
       </c>
       <c r="X136" s="19">
-        <f>R136/50*1000*10^3</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y136" s="19">
-        <f>S136/50*1000*10^4</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>19600000</v>
       </c>
       <c r="Z136" s="19">
-        <f>T136/50*1000*10^5</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>10000000</v>
       </c>
       <c r="AA136" s="19">
-        <f>U136/50*1000*10^3</f>
+        <f t="shared" si="4"/>
         <v>7240000</v>
       </c>
       <c r="AB136" s="19">
-        <f>V136/50*1000*10^4</f>
+        <f t="shared" si="5"/>
         <v>11200000</v>
       </c>
       <c r="AC136" s="19">
-        <f>W136/50*1000*10^5</f>
+        <f t="shared" si="6"/>
         <v>14000000</v>
       </c>
-      <c r="AD136" s="19" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+      <c r="AD136" s="6">
+        <f>AA136*K136/(Y136*7)</f>
+        <v>0.19192860058309039</v>
       </c>
     </row>
     <row r="137" spans="1:30" x14ac:dyDescent="0.3">
@@ -8229,6 +8302,12 @@
       <c r="L137" s="9">
         <v>1E-3</v>
       </c>
+      <c r="S137">
+        <v>89</v>
+      </c>
+      <c r="T137">
+        <v>8</v>
+      </c>
       <c r="U137">
         <v>404</v>
       </c>
@@ -8239,32 +8318,32 @@
         <v>5</v>
       </c>
       <c r="X137" s="19">
-        <f>R137/50*1000*10^3</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y137" s="19">
-        <f>S137/50*1000*10^4</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>17800000</v>
       </c>
       <c r="Z137" s="19">
-        <f>T137/50*1000*10^5</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>16000000</v>
       </c>
       <c r="AA137" s="19">
-        <f>U137/50*1000*10^3</f>
+        <f t="shared" si="4"/>
         <v>8080000</v>
       </c>
       <c r="AB137" s="19">
-        <f>V137/50*1000*10^4</f>
+        <f t="shared" si="5"/>
         <v>12000000</v>
       </c>
       <c r="AC137" s="19">
-        <f>W137/50*1000*10^5</f>
+        <f t="shared" si="6"/>
         <v>10000000</v>
       </c>
-      <c r="AD137" s="19" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+      <c r="AD137" s="6">
+        <f t="shared" si="9"/>
+        <v>0.2686048796147672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: spinning, plasma film, HEPES dilution viscosity data
</commit_message>
<xml_diff>
--- a/Data-analysis/Spinning.xlsx
+++ b/Data-analysis/Spinning.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D218B502-5D7D-49A9-A65F-E248D68764CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22272" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22275" windowHeight="13170" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main_page_wide" sheetId="1" r:id="rId1"/>
     <sheet name="Hematocrit" sheetId="3" r:id="rId2"/>
     <sheet name="Bad data" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="J31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="J31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O93" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="O93" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P93" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="P93" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q93" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="Q93" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -131,12 +130,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="J3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -165,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="85">
   <si>
     <t>Disk</t>
   </si>
@@ -412,11 +411,20 @@
   <si>
     <t>c_spin-5</t>
   </si>
+  <si>
+    <t>Moat2_glossy</t>
+  </si>
+  <si>
+    <t>20.05_8x3_1.25x7mm</t>
+  </si>
+  <si>
+    <t>20.05_8x3_1.25x9mm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -517,7 +525,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -691,12 +699,15 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D7BE-4BB3-83A6-8706B9602D6E}"/>
+            </c:ext>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredSeriesTitle>
                 <c15:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!#REF!</c15:sqref>
@@ -713,9 +724,6 @@
                 </c15:tx>
               </c15:filteredSeriesTitle>
             </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D7BE-4BB3-83A6-8706B9602D6E}"/>
-            </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
@@ -726,11 +734,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1453056192"/>
-        <c:axId val="-1453048032"/>
+        <c:axId val="1476999520"/>
+        <c:axId val="1477000608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1453056192"/>
+        <c:axId val="1476999520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,12 +850,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1453048032"/>
+        <c:crossAx val="1477000608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1453048032"/>
+        <c:axId val="1477000608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -959,7 +967,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1453056192"/>
+        <c:crossAx val="1476999520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -973,14 +981,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1591,7 +1599,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBFBBC99-885F-4EF6-B984-4882307E780A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CBFBBC99-885F-4EF6-B984-4882307E780A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1635,7 +1643,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4346EC53-EF7D-4616-BDFA-5D8CA0D5F4BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4346EC53-EF7D-4616-BDFA-5D8CA0D5F4BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1679,7 +1687,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A121844-DCEF-493C-B950-93833269643C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4A121844-DCEF-493C-B950-93833269643C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1723,7 +1731,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3493C57-AF06-4E58-AE0A-802C6FD0D299}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F3493C57-AF06-4E58-AE0A-802C6FD0D299}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1773,7 +1781,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F423840-B72F-4217-9ED7-6AC9B7BDACE9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6F423840-B72F-4217-9ED7-6AC9B7BDACE9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1823,7 +1831,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C7C2062-9BD2-442C-85A1-AC7A4EB0E37A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7C7C2062-9BD2-442C-85A1-AC7A4EB0E37A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1920,23 +1928,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1972,23 +1963,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2164,28 +2138,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="I8" sqref="I8:I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="7" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2235,7 +2209,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43242</v>
       </c>
@@ -2255,7 +2229,7 @@
         <v>4.0156999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43242</v>
       </c>
@@ -2275,7 +2249,7 @@
         <v>3.9187999999999992</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43242</v>
       </c>
@@ -2298,7 +2272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43242</v>
       </c>
@@ -2318,7 +2292,7 @@
         <v>4.8489000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43242</v>
       </c>
@@ -2338,7 +2312,7 @@
         <v>3.5714999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43242</v>
       </c>
@@ -2358,7 +2332,7 @@
         <v>4.0186999999999991</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43258</v>
       </c>
@@ -2407,7 +2381,7 @@
         <v>6.7259070000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43258</v>
       </c>
@@ -2455,7 +2429,7 @@
         <v>3.1300000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43258</v>
       </c>
@@ -2503,7 +2477,7 @@
         <v>1.5699999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43258</v>
       </c>
@@ -2551,7 +2525,7 @@
         <v>0.98429999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43258</v>
       </c>
@@ -2587,7 +2561,7 @@
         <v>3.07</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43258</v>
       </c>
@@ -2623,7 +2597,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43258</v>
       </c>
@@ -2666,7 +2640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43258</v>
       </c>
@@ -2703,7 +2677,7 @@
         <v>4.4399999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43264</v>
       </c>
@@ -2730,7 +2704,7 @@
         <v>3.1424000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43264</v>
       </c>
@@ -2757,7 +2731,7 @@
         <v>3.8690000000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43264</v>
       </c>
@@ -2793,7 +2767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43264</v>
       </c>
@@ -2836,7 +2810,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43264</v>
       </c>
@@ -2880,7 +2854,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43264</v>
       </c>
@@ -2923,7 +2897,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="P22" s="2">
@@ -2936,7 +2910,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="P23" s="2">
@@ -2949,7 +2923,7 @@
         <v>49.23</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="P24" s="2">
@@ -2962,7 +2936,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="P25" s="2">
@@ -2975,7 +2949,7 @@
         <v>48.43</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="P26" s="2">
@@ -2988,7 +2962,7 @@
         <v>49.62</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="H27" s="4"/>
@@ -3002,7 +2976,7 @@
         <v>50.77</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="P28" s="2">
@@ -3015,7 +2989,7 @@
         <v>49.25</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="P29" s="2">
@@ -3028,7 +3002,7 @@
         <v>46.04</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="P30" s="2">
@@ -3041,7 +3015,7 @@
         <v>49.23</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="P31" s="2">
@@ -3061,7 +3035,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="P32" s="2">
@@ -3081,7 +3055,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="P33" s="2">
@@ -3101,7 +3075,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="P34" s="2">
@@ -3114,7 +3088,7 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="P35" s="2">
@@ -3127,7 +3101,7 @@
         <v>3.07</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="P36" s="2">
@@ -3140,7 +3114,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="P37" s="2">
@@ -3153,7 +3127,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="P38" s="2">
@@ -3166,7 +3140,7 @@
         <v>3.27</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="P39" s="2">
@@ -3179,7 +3153,7 @@
         <v>3.07</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="P40" s="2">
@@ -3192,7 +3166,7 @@
         <v>3.07</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="P41" s="2">
@@ -3205,7 +3179,7 @@
         <v>3.68</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P42" s="2">
         <v>6</v>
       </c>
@@ -3223,33 +3197,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AD137"/>
+  <dimension ref="A1:AD149"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z131" sqref="Z131"/>
+      <selection pane="bottomLeft" activeCell="K138" sqref="K138:K149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" customWidth="1"/>
-    <col min="7" max="10" width="8.88671875" style="6"/>
-    <col min="11" max="11" width="8.88671875" style="10"/>
-    <col min="12" max="12" width="8.88671875" style="9"/>
-    <col min="13" max="14" width="9.109375" style="9"/>
-    <col min="15" max="16" width="8.88671875" style="10"/>
-    <col min="18" max="18" width="8.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" customWidth="1"/>
+    <col min="7" max="10" width="8.85546875" style="6"/>
+    <col min="11" max="11" width="8.85546875" style="10"/>
+    <col min="12" max="12" width="8.85546875" style="9"/>
+    <col min="13" max="14" width="9.140625" style="9"/>
+    <col min="15" max="16" width="8.85546875" style="10"/>
+    <col min="18" max="18" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="24" max="29" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -3341,7 +3315,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43242</v>
       </c>
@@ -3392,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43242</v>
       </c>
@@ -3418,7 +3392,7 @@
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43242</v>
       </c>
@@ -3444,7 +3418,7 @@
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43242</v>
       </c>
@@ -3470,7 +3444,7 @@
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43242</v>
       </c>
@@ -3496,7 +3470,7 @@
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43242</v>
       </c>
@@ -3522,7 +3496,7 @@
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43258</v>
       </c>
@@ -3562,7 +3536,7 @@
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43258</v>
       </c>
@@ -3601,7 +3575,7 @@
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43258</v>
       </c>
@@ -3640,7 +3614,7 @@
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43258</v>
       </c>
@@ -3679,7 +3653,7 @@
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43258</v>
       </c>
@@ -3718,7 +3692,7 @@
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43258</v>
       </c>
@@ -3757,7 +3731,7 @@
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43258</v>
       </c>
@@ -3796,7 +3770,7 @@
       <c r="O14" s="9"/>
       <c r="P14" s="9"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43258</v>
       </c>
@@ -3835,7 +3809,7 @@
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43264</v>
       </c>
@@ -3868,7 +3842,7 @@
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43264</v>
       </c>
@@ -3901,7 +3875,7 @@
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43264</v>
       </c>
@@ -3934,7 +3908,7 @@
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43264</v>
       </c>
@@ -3967,7 +3941,7 @@
       <c r="O19" s="9"/>
       <c r="P19" s="9"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43264</v>
       </c>
@@ -4003,7 +3977,7 @@
       <c r="O20" s="9"/>
       <c r="P20" s="9"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43264</v>
       </c>
@@ -4036,7 +4010,7 @@
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43293</v>
       </c>
@@ -4062,7 +4036,7 @@
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43298</v>
       </c>
@@ -4092,7 +4066,7 @@
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43298</v>
       </c>
@@ -4122,7 +4096,7 @@
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43298</v>
       </c>
@@ -4152,7 +4126,7 @@
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43298</v>
       </c>
@@ -4182,7 +4156,7 @@
       <c r="O26" s="9"/>
       <c r="P26" s="9"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43298</v>
       </c>
@@ -4213,7 +4187,7 @@
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43298</v>
       </c>
@@ -4243,7 +4217,7 @@
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43305</v>
       </c>
@@ -4273,7 +4247,7 @@
       <c r="O29" s="9"/>
       <c r="P29" s="9"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43305</v>
       </c>
@@ -4303,7 +4277,7 @@
       <c r="O30" s="9"/>
       <c r="P30" s="9"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43305</v>
       </c>
@@ -4337,7 +4311,7 @@
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43305</v>
       </c>
@@ -4371,7 +4345,7 @@
       <c r="O32" s="9"/>
       <c r="P32" s="9"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43305</v>
       </c>
@@ -4401,7 +4375,7 @@
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43305</v>
       </c>
@@ -4431,7 +4405,7 @@
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43305</v>
       </c>
@@ -4461,7 +4435,7 @@
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43305</v>
       </c>
@@ -4491,7 +4465,7 @@
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43307</v>
       </c>
@@ -4522,7 +4496,7 @@
       <c r="O37" s="9"/>
       <c r="P37" s="9"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43307</v>
       </c>
@@ -4553,7 +4527,7 @@
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43307</v>
       </c>
@@ -4584,7 +4558,7 @@
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43307</v>
       </c>
@@ -4615,7 +4589,7 @@
       <c r="O40" s="9"/>
       <c r="P40" s="9"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43312</v>
       </c>
@@ -4645,7 +4619,7 @@
       <c r="O41" s="9"/>
       <c r="P41" s="9"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43312</v>
       </c>
@@ -4675,7 +4649,7 @@
       <c r="O42" s="9"/>
       <c r="P42" s="9"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43312</v>
       </c>
@@ -4705,7 +4679,7 @@
       <c r="O43" s="9"/>
       <c r="P43" s="9"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43312</v>
       </c>
@@ -4735,7 +4709,7 @@
       <c r="O44" s="9"/>
       <c r="P44" s="9"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43312</v>
       </c>
@@ -4765,7 +4739,7 @@
       <c r="O45" s="9"/>
       <c r="P45" s="9"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43312</v>
       </c>
@@ -4795,7 +4769,7 @@
       <c r="O46" s="9"/>
       <c r="P46" s="9"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43312</v>
       </c>
@@ -4825,7 +4799,7 @@
       <c r="O47" s="9"/>
       <c r="P47" s="9"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43314</v>
       </c>
@@ -4855,7 +4829,7 @@
       <c r="O48" s="9"/>
       <c r="P48" s="9"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43314</v>
       </c>
@@ -4885,7 +4859,7 @@
       <c r="O49" s="9"/>
       <c r="P49" s="9"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43314</v>
       </c>
@@ -4915,7 +4889,7 @@
       <c r="O50" s="9"/>
       <c r="P50" s="9"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43314</v>
       </c>
@@ -4945,7 +4919,7 @@
       <c r="O51" s="9"/>
       <c r="P51" s="9"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43314</v>
       </c>
@@ -4975,7 +4949,7 @@
       <c r="O52" s="9"/>
       <c r="P52" s="9"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43314</v>
       </c>
@@ -5005,7 +4979,7 @@
       <c r="O53" s="9"/>
       <c r="P53" s="9"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43314</v>
       </c>
@@ -5035,7 +5009,7 @@
       <c r="O54" s="9"/>
       <c r="P54" s="9"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43314</v>
       </c>
@@ -5065,7 +5039,7 @@
       <c r="O55" s="9"/>
       <c r="P55" s="9"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43319</v>
       </c>
@@ -5095,7 +5069,7 @@
       <c r="O56" s="9"/>
       <c r="P56" s="9"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43319</v>
       </c>
@@ -5125,7 +5099,7 @@
       <c r="O57" s="9"/>
       <c r="P57" s="9"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43319</v>
       </c>
@@ -5155,7 +5129,7 @@
       <c r="O58" s="9"/>
       <c r="P58" s="9"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43319</v>
       </c>
@@ -5185,7 +5159,7 @@
       <c r="O59" s="9"/>
       <c r="P59" s="9"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43319</v>
       </c>
@@ -5215,7 +5189,7 @@
       <c r="O60" s="9"/>
       <c r="P60" s="9"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43319</v>
       </c>
@@ -5242,7 +5216,7 @@
       <c r="O61" s="9"/>
       <c r="P61" s="9"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43321</v>
       </c>
@@ -5275,7 +5249,7 @@
       <c r="O62" s="9"/>
       <c r="P62" s="9"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43321</v>
       </c>
@@ -5308,7 +5282,7 @@
       <c r="O63" s="9"/>
       <c r="P63" s="9"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43321</v>
       </c>
@@ -5341,7 +5315,7 @@
       <c r="O64" s="9"/>
       <c r="P64" s="9"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43321</v>
       </c>
@@ -5374,7 +5348,7 @@
       <c r="O65" s="9"/>
       <c r="P65" s="9"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>43321</v>
       </c>
@@ -5407,7 +5381,7 @@
       <c r="O66" s="9"/>
       <c r="P66" s="9"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>43321</v>
       </c>
@@ -5440,7 +5414,7 @@
       <c r="O67" s="9"/>
       <c r="P67" s="9"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>43321</v>
       </c>
@@ -5473,7 +5447,7 @@
       <c r="O68" s="9"/>
       <c r="P68" s="9"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>43326</v>
       </c>
@@ -5506,7 +5480,7 @@
       <c r="O69" s="9"/>
       <c r="P69" s="9"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>43326</v>
       </c>
@@ -5539,7 +5513,7 @@
       <c r="O70" s="9"/>
       <c r="P70" s="9"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>43326</v>
       </c>
@@ -5572,7 +5546,7 @@
       <c r="O71" s="9"/>
       <c r="P71" s="9"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>43326</v>
       </c>
@@ -5605,7 +5579,7 @@
       <c r="O72" s="9"/>
       <c r="P72" s="9"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>43326</v>
       </c>
@@ -5639,7 +5613,7 @@
       <c r="O73" s="9"/>
       <c r="P73" s="9"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>43326</v>
       </c>
@@ -5669,7 +5643,7 @@
       <c r="O74" s="9"/>
       <c r="P74" s="9"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>43326</v>
       </c>
@@ -5702,7 +5676,7 @@
       <c r="O75" s="9"/>
       <c r="P75" s="9"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>43328</v>
       </c>
@@ -5735,7 +5709,7 @@
       <c r="O76" s="9"/>
       <c r="P76" s="9"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>43328</v>
       </c>
@@ -5768,7 +5742,7 @@
       <c r="O77" s="9"/>
       <c r="P77" s="9"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>43328</v>
       </c>
@@ -5801,7 +5775,7 @@
       <c r="O78" s="9"/>
       <c r="P78" s="9"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>43328</v>
       </c>
@@ -5834,7 +5808,7 @@
       <c r="O79" s="9"/>
       <c r="P79" s="9"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>43328</v>
       </c>
@@ -5867,7 +5841,7 @@
       <c r="O80" s="9"/>
       <c r="P80" s="9"/>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>43328</v>
       </c>
@@ -5900,7 +5874,7 @@
       <c r="O81" s="9"/>
       <c r="P81" s="9"/>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>43328</v>
       </c>
@@ -5933,7 +5907,7 @@
       <c r="O82" s="9"/>
       <c r="P82" s="9"/>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>43328</v>
       </c>
@@ -5966,7 +5940,7 @@
       <c r="O83" s="9"/>
       <c r="P83" s="9"/>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>43328</v>
       </c>
@@ -5999,7 +5973,7 @@
       <c r="O84" s="9"/>
       <c r="P84" s="9"/>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>43328</v>
       </c>
@@ -6029,7 +6003,7 @@
       <c r="O85" s="9"/>
       <c r="P85" s="9"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>43333</v>
       </c>
@@ -6069,7 +6043,7 @@
         <v>4.6127000000000038</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>43333</v>
       </c>
@@ -6109,7 +6083,7 @@
         <v>4.5798000000000059</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>43333</v>
       </c>
@@ -6149,7 +6123,7 @@
         <v>4.6700000000000017</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>43333</v>
       </c>
@@ -6189,7 +6163,7 @@
         <v>4.7094000000000023</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>43333</v>
       </c>
@@ -6229,7 +6203,7 @@
         <v>4.6321000000000083</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>43333</v>
       </c>
@@ -6263,7 +6237,7 @@
       </c>
       <c r="Q91" s="10"/>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>43334</v>
       </c>
@@ -6294,7 +6268,7 @@
       </c>
       <c r="Q92" s="10"/>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>43334</v>
       </c>
@@ -6334,7 +6308,7 @@
         <v>4.4594999999999914</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>43334</v>
       </c>
@@ -6374,7 +6348,7 @@
         <v>4.3830999999999989</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>43334</v>
       </c>
@@ -6414,7 +6388,7 @@
         <v>4.4004999999999939</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>43334</v>
       </c>
@@ -6454,7 +6428,7 @@
         <v>4.3624999999999972</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>43334</v>
       </c>
@@ -6494,7 +6468,7 @@
         <v>4.3070999999999913</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>43340</v>
       </c>
@@ -6537,7 +6511,7 @@
         <v>4.4329000000000036</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>43340</v>
       </c>
@@ -6580,7 +6554,7 @@
         <v>4.3871999999999929</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>43340</v>
       </c>
@@ -6623,7 +6597,7 @@
         <v>4.4403999999999968</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>43340</v>
       </c>
@@ -6660,7 +6634,7 @@
       </c>
       <c r="S101" s="10"/>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>43340</v>
       </c>
@@ -6700,7 +6674,7 @@
         <v>4.4458999999999946</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>43340</v>
       </c>
@@ -6740,7 +6714,7 @@
         <v>4.4919000000000011</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>43340</v>
       </c>
@@ -6783,7 +6757,7 @@
         <v>4.4684000000000026</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>43342</v>
       </c>
@@ -6816,7 +6790,7 @@
         <v>0.80500000000000005</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>43342</v>
       </c>
@@ -6849,7 +6823,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>43342</v>
       </c>
@@ -6882,7 +6856,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>43342</v>
       </c>
@@ -6915,7 +6889,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>43342</v>
       </c>
@@ -6948,7 +6922,7 @@
         <v>0.86499999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>43342</v>
       </c>
@@ -6981,7 +6955,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>43349</v>
       </c>
@@ -7017,7 +6991,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>43349</v>
       </c>
@@ -7053,7 +7027,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="113" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>43349</v>
       </c>
@@ -7089,7 +7063,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="114" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>43349</v>
       </c>
@@ -7125,7 +7099,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="115" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>43564</v>
       </c>
@@ -7154,7 +7128,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="116" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>43564</v>
       </c>
@@ -7183,7 +7157,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>43564</v>
       </c>
@@ -7212,7 +7186,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="118" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>43564</v>
       </c>
@@ -7241,7 +7215,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="119" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>43564</v>
       </c>
@@ -7270,7 +7244,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="120" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>43564</v>
       </c>
@@ -7299,7 +7273,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>43564</v>
       </c>
@@ -7328,7 +7302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>43564</v>
       </c>
@@ -7357,7 +7331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>43564</v>
       </c>
@@ -7386,7 +7360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>43564</v>
       </c>
@@ -7415,7 +7389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="14">
         <v>43564</v>
       </c>
@@ -7452,7 +7426,7 @@
       <c r="P125" s="18"/>
       <c r="R125" s="18"/>
     </row>
-    <row r="126" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>43571</v>
       </c>
@@ -7526,7 +7500,7 @@
         <v>0.10268858338314407</v>
       </c>
     </row>
-    <row r="127" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>43571</v>
       </c>
@@ -7572,7 +7546,7 @@
         <v>4</v>
       </c>
       <c r="X127" s="19">
-        <f t="shared" ref="X126:X137" si="7">R127/50*1000*10^3</f>
+        <f t="shared" ref="X127:X137" si="7">R127/50*1000*10^3</f>
         <v>0</v>
       </c>
       <c r="Y127" s="19">
@@ -7600,7 +7574,7 @@
         <v>0.13901456310679611</v>
       </c>
     </row>
-    <row r="128" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>43571</v>
       </c>
@@ -7674,7 +7648,7 @@
         <v>0.10428121118012422</v>
       </c>
     </row>
-    <row r="129" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>43571</v>
       </c>
@@ -7748,7 +7722,7 @@
         <v>0.11624593886462879</v>
       </c>
     </row>
-    <row r="130" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>43571</v>
       </c>
@@ -7825,7 +7799,7 @@
         <v>0.12834833976833979</v>
       </c>
     </row>
-    <row r="131" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>43571</v>
       </c>
@@ -7902,7 +7876,7 @@
         <v>0.13307666666666665</v>
       </c>
     </row>
-    <row r="132" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>43571</v>
       </c>
@@ -7976,7 +7950,7 @@
         <v>0.18145821138211382</v>
       </c>
     </row>
-    <row r="133" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>43571</v>
       </c>
@@ -8050,7 +8024,7 @@
         <v>0.34329004264392315</v>
       </c>
     </row>
-    <row r="134" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>43571</v>
       </c>
@@ -8124,7 +8098,7 @@
         <v>0.54445186813186808</v>
       </c>
     </row>
-    <row r="135" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>43571</v>
       </c>
@@ -8198,7 +8172,7 @@
         <v>0.30591914285714278</v>
       </c>
     </row>
-    <row r="136" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>43571</v>
       </c>
@@ -8272,7 +8246,7 @@
         <v>0.19192860058309039</v>
       </c>
     </row>
-    <row r="137" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>43571</v>
       </c>
@@ -8344,6 +8318,369 @@
       <c r="AD137" s="6">
         <f t="shared" si="9"/>
         <v>0.2686048796147672</v>
+      </c>
+    </row>
+    <row r="138" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B138" s="2">
+        <v>1</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D138" t="s">
+        <v>83</v>
+      </c>
+      <c r="E138">
+        <v>4</v>
+      </c>
+      <c r="F138" t="s">
+        <v>7</v>
+      </c>
+      <c r="G138" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K138" s="10">
+        <f>10.0224-6.1343</f>
+        <v>3.8880999999999997</v>
+      </c>
+      <c r="L138" s="9">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B139" s="2">
+        <v>2</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D139" t="s">
+        <v>82</v>
+      </c>
+      <c r="E139">
+        <v>4</v>
+      </c>
+      <c r="F139" t="s">
+        <v>7</v>
+      </c>
+      <c r="G139" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K139" s="10">
+        <f>9.2132-6.0331</f>
+        <v>3.1801000000000004</v>
+      </c>
+      <c r="L139" s="9">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B140" s="2">
+        <v>3</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D140" t="s">
+        <v>84</v>
+      </c>
+      <c r="E140">
+        <v>4</v>
+      </c>
+      <c r="F140" t="s">
+        <v>7</v>
+      </c>
+      <c r="G140" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K140" s="10">
+        <f>9.7443-6.0381</f>
+        <v>3.7062000000000008</v>
+      </c>
+      <c r="L140" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B141" s="2">
+        <v>4</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D141" t="s">
+        <v>83</v>
+      </c>
+      <c r="E141">
+        <v>4</v>
+      </c>
+      <c r="F141" t="s">
+        <v>7</v>
+      </c>
+      <c r="G141" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K141" s="10">
+        <f>10.2184-6.1569</f>
+        <v>4.0615000000000006</v>
+      </c>
+      <c r="L141" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B142" s="2">
+        <v>5</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D142" t="s">
+        <v>82</v>
+      </c>
+      <c r="E142">
+        <v>4</v>
+      </c>
+      <c r="F142" t="s">
+        <v>7</v>
+      </c>
+      <c r="G142" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K142" s="10">
+        <f>9.4637-6.0543</f>
+        <v>3.4093999999999998</v>
+      </c>
+      <c r="L142" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B143" s="2">
+        <v>6</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D143" t="s">
+        <v>84</v>
+      </c>
+      <c r="E143">
+        <v>4</v>
+      </c>
+      <c r="F143" t="s">
+        <v>7</v>
+      </c>
+      <c r="G143" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K143" s="10">
+        <f>9.9504-6.0779</f>
+        <v>3.8725000000000005</v>
+      </c>
+      <c r="L143" s="9">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B144" s="2">
+        <v>1</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D144" t="s">
+        <v>83</v>
+      </c>
+      <c r="E144">
+        <v>4</v>
+      </c>
+      <c r="F144" t="s">
+        <v>49</v>
+      </c>
+      <c r="G144" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="I144"/>
+      <c r="K144" s="10">
+        <f>10.2134-6.014</f>
+        <v>4.1993999999999998</v>
+      </c>
+      <c r="L144" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B145" s="2">
+        <v>2</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D145" t="s">
+        <v>84</v>
+      </c>
+      <c r="E145">
+        <v>4</v>
+      </c>
+      <c r="F145" t="s">
+        <v>49</v>
+      </c>
+      <c r="G145" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="I145"/>
+      <c r="K145" s="10">
+        <f>10.2447-6.1587</f>
+        <v>4.0860000000000003</v>
+      </c>
+      <c r="L145" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B146" s="2">
+        <v>3</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D146" t="s">
+        <v>82</v>
+      </c>
+      <c r="E146">
+        <v>4</v>
+      </c>
+      <c r="F146" t="s">
+        <v>49</v>
+      </c>
+      <c r="G146" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="I146"/>
+      <c r="K146" s="10">
+        <f>8.9526-6.0303</f>
+        <v>2.9222999999999999</v>
+      </c>
+      <c r="L146" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B147" s="2">
+        <v>4</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D147" t="s">
+        <v>83</v>
+      </c>
+      <c r="E147">
+        <v>4</v>
+      </c>
+      <c r="F147" t="s">
+        <v>49</v>
+      </c>
+      <c r="G147" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="K147" s="10">
+        <f>10.2938-6.0305</f>
+        <v>4.2632999999999992</v>
+      </c>
+      <c r="L147" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B148" s="2">
+        <v>5</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D148" t="s">
+        <v>84</v>
+      </c>
+      <c r="E148">
+        <v>4</v>
+      </c>
+      <c r="F148" t="s">
+        <v>49</v>
+      </c>
+      <c r="G148" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="K148" s="10">
+        <f>10.161-6.1216</f>
+        <v>4.0393999999999997</v>
+      </c>
+      <c r="L148" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B149" s="2">
+        <v>6</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D149" t="s">
+        <v>82</v>
+      </c>
+      <c r="E149">
+        <v>4</v>
+      </c>
+      <c r="F149" t="s">
+        <v>49</v>
+      </c>
+      <c r="G149" s="6">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="K149" s="10">
+        <f>9.5773-6.0861</f>
+        <v>3.4911999999999992</v>
+      </c>
+      <c r="L149" s="9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8353,7 +8690,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O6"/>
   <sheetViews>
@@ -8361,12 +8698,12 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -8413,7 +8750,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43249</v>
       </c>
@@ -8456,7 +8793,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43249</v>
       </c>
@@ -8483,7 +8820,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43249</v>
       </c>
@@ -8511,7 +8848,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43249</v>
       </c>
@@ -8539,7 +8876,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43249</v>
       </c>

</xml_diff>